<commit_message>
Dropdown from row 2 instead of 1 and demo 15_03
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_03.w3mi.data.xlsx
+++ b/src/zdemo_excel15_03.w3mi.data.xlsx
@@ -417,7 +417,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" zoomScaleSheetLayoutView="100" workbookViewId="0" showGridLines="1" showRowColHeaders="1">
-      <pane ySplit="3" xSplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane ySplit="1" xSplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1465,7 +1465,7 @@
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" ShowDropDown="1" errorStyle="stop" sqref="C4">
+    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" ShowDropDown="1" errorStyle="stop" sqref="A2:A1048576">
       <formula1>Airlines</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
partial fix for issue 12 (#41)
Fix #12 
* partial fix for issue 12
* updated corresponding reference file
* Dropdown from row 2 instead of 1 and demo 15_03
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_03.w3mi.data.xlsx
+++ b/src/zdemo_excel15_03.w3mi.data.xlsx
@@ -417,7 +417,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" zoomScaleSheetLayoutView="100" workbookViewId="0" showGridLines="1" showRowColHeaders="1">
-      <pane ySplit="3" xSplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane ySplit="1" xSplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1465,7 +1465,7 @@
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" ShowDropDown="1" errorStyle="stop" sqref="C4">
+    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" ShowDropDown="1" errorStyle="stop" sqref="A2:A1048576">
       <formula1>Airlines</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changed Excel file for ZDEMO_EXCEL15_03
Fix #48
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_03.w3mi.data.xlsx
+++ b/src/zdemo_excel15_03.w3mi.data.xlsx
@@ -150,6 +150,28 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="table1" displayName="table1" ref="A1:M25" totalsRowShown="0">
+  <autoFilter ref="A1:M25"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Airline"/>
+    <tableColumn id="2" name="Flight Number"/>
+    <tableColumn id="3" name="Date"/>
+    <tableColumn id="4" name="Airfare"/>
+    <tableColumn id="5" name="Airline Currency"/>
+    <tableColumn id="6" name="Plane Type"/>
+    <tableColumn id="7" name="Max. capacity econ."/>
+    <tableColumn id="8" name="Occupied econ."/>
+    <tableColumn id="9" name="Total"/>
+    <tableColumn id="10" name="Max. capacity bus."/>
+    <tableColumn id="11" name="Occupied bus."/>
+    <tableColumn id="12" name="Max. capacity 1st"/>
+    <tableColumn id="13" name="Occupied 1st"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1474,6 +1496,9 @@
   <ignoredErrors>
     <ignoredError sqref="B2:B25" numberStoredAsText="1"/>
   </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed Excel file for ZDEMO_EXCEL15_03 (#49)
Fix #48
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_03.w3mi.data.xlsx
+++ b/src/zdemo_excel15_03.w3mi.data.xlsx
@@ -150,6 +150,28 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="table1" displayName="table1" ref="A1:M25" totalsRowShown="0">
+  <autoFilter ref="A1:M25"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Airline"/>
+    <tableColumn id="2" name="Flight Number"/>
+    <tableColumn id="3" name="Date"/>
+    <tableColumn id="4" name="Airfare"/>
+    <tableColumn id="5" name="Airline Currency"/>
+    <tableColumn id="6" name="Plane Type"/>
+    <tableColumn id="7" name="Max. capacity econ."/>
+    <tableColumn id="8" name="Occupied econ."/>
+    <tableColumn id="9" name="Total"/>
+    <tableColumn id="10" name="Max. capacity bus."/>
+    <tableColumn id="11" name="Occupied bus."/>
+    <tableColumn id="12" name="Max. capacity 1st"/>
+    <tableColumn id="13" name="Occupied 1st"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1474,6 +1496,9 @@
   <ignoredErrors>
     <ignoredError sqref="B2:B25" numberStoredAsText="1"/>
   </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>